<commit_message>
Refactoring WebAutomation; download metadata from first page results of each query
</commit_message>
<xml_diff>
--- a/Source/NetworkStuff/WebAutomation/Book1.xlsx
+++ b/Source/NetworkStuff/WebAutomation/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\theok\Repos\FactCheckThisBitch\Source\NetworkStuff\WebAutomation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDC9B73-FB8D-4B88-8CF0-38D2F0B22F4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85AFEF07-3449-4089-8DEB-3620DF0B0E34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F78B371-5E18-40C2-992A-732B5DD7542A}"/>
   </bookViews>
@@ -350,154 +350,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>150</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>112</c:v>
+                  <c:v>111</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>184</c:v>
+                  <c:v>115</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149</c:v>
+                  <c:v>154</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>165</c:v>
+                  <c:v>161</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>143</c:v>
+                  <c:v>146</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>184</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>165</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="10">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>149</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>207</c:v>
+                </c:pt>
+                <c:pt idx="13">
                   <c:v>80</c:v>
                 </c:pt>
-                <c:pt idx="11">
-                  <c:v>283</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="14">
+                  <c:v>210</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>167</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>88</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>253</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>339</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>299</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>248</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>230</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="33">
                   <c:v>145</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>166</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>168</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>306</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>175</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>315</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>262</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>77</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>332</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>193</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>202</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>118</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>260</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>39</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>88</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>236</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>145</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>112</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>136</c:v>
-                </c:pt>
                 <c:pt idx="34">
-                  <c:v>194</c:v>
+                  <c:v>123</c:v>
                 </c:pt>
                 <c:pt idx="35">
                   <c:v>126</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>69</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>121</c:v>
+                  <c:v>127</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>129</c:v>
+                  <c:v>150</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>125</c:v>
+                  <c:v>212</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>339</c:v>
+                  <c:v>207</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>315</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>168</c:v>
+                  <c:v>157</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>225</c:v>
+                  <c:v>205</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>232</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>308</c:v>
+                  <c:v>323</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>123</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>98</c:v>
+                  <c:v>141</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>209</c:v>
+                  <c:v>180</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -735,7 +735,7 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -768,7 +768,7 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>4</c:v>
@@ -777,7 +777,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>1</c:v>
@@ -828,13 +828,13 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>8</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="34">
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>2</c:v>
@@ -858,7 +858,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="44">
                   <c:v>7</c:v>
@@ -873,7 +873,7 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>27</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>10</c:v>
@@ -1057,6 +1057,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1248360288"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -2011,7 +2012,7 @@
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2042,7 +2043,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>150</v>
+        <v>100</v>
       </c>
       <c r="C2">
         <v>4</v>
@@ -2053,7 +2054,7 @@
         <v>43132</v>
       </c>
       <c r="B3">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -2064,10 +2065,10 @@
         <v>43160</v>
       </c>
       <c r="B4">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -2075,7 +2076,7 @@
         <v>43191</v>
       </c>
       <c r="B5">
-        <v>184</v>
+        <v>115</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -2086,7 +2087,7 @@
         <v>43221</v>
       </c>
       <c r="B6">
-        <v>149</v>
+        <v>154</v>
       </c>
       <c r="C6">
         <v>2</v>
@@ -2097,7 +2098,7 @@
         <v>43252</v>
       </c>
       <c r="B7">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -2119,7 +2120,7 @@
         <v>43313</v>
       </c>
       <c r="B9">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -2130,7 +2131,7 @@
         <v>43344</v>
       </c>
       <c r="B10">
-        <v>184</v>
+        <v>204</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -2141,7 +2142,7 @@
         <v>43374</v>
       </c>
       <c r="B11">
-        <v>165</v>
+        <v>236</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -2152,7 +2153,7 @@
         <v>43405</v>
       </c>
       <c r="B12">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -2163,7 +2164,7 @@
         <v>43435</v>
       </c>
       <c r="B13">
-        <v>283</v>
+        <v>149</v>
       </c>
       <c r="C13">
         <v>1</v>
@@ -2174,7 +2175,7 @@
         <v>43466</v>
       </c>
       <c r="B14">
-        <v>145</v>
+        <v>207</v>
       </c>
       <c r="C14">
         <v>2</v>
@@ -2185,10 +2186,10 @@
         <v>43497</v>
       </c>
       <c r="B15">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="C15">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -2196,7 +2197,7 @@
         <v>43525</v>
       </c>
       <c r="B16">
-        <v>166</v>
+        <v>210</v>
       </c>
       <c r="C16">
         <v>4</v>
@@ -2207,7 +2208,7 @@
         <v>43556</v>
       </c>
       <c r="B17">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -2218,10 +2219,10 @@
         <v>43586</v>
       </c>
       <c r="B18">
-        <v>306</v>
+        <v>170</v>
       </c>
       <c r="C18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2229,7 +2230,7 @@
         <v>43617</v>
       </c>
       <c r="B19">
-        <v>118</v>
+        <v>88</v>
       </c>
       <c r="C19">
         <v>1</v>
@@ -2240,7 +2241,7 @@
         <v>43647</v>
       </c>
       <c r="B20">
-        <v>175</v>
+        <v>253</v>
       </c>
       <c r="C20">
         <v>2</v>
@@ -2251,7 +2252,7 @@
         <v>43678</v>
       </c>
       <c r="B21">
-        <v>315</v>
+        <v>339</v>
       </c>
       <c r="C21">
         <v>7</v>
@@ -2262,7 +2263,7 @@
         <v>43709</v>
       </c>
       <c r="B22">
-        <v>262</v>
+        <v>299</v>
       </c>
       <c r="C22">
         <v>0</v>
@@ -2273,7 +2274,7 @@
         <v>43739</v>
       </c>
       <c r="B23">
-        <v>77</v>
+        <v>112</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -2284,7 +2285,7 @@
         <v>43770</v>
       </c>
       <c r="B24">
-        <v>332</v>
+        <v>172</v>
       </c>
       <c r="C24">
         <v>7</v>
@@ -2295,7 +2296,7 @@
         <v>43800</v>
       </c>
       <c r="B25">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -2306,7 +2307,7 @@
         <v>43831</v>
       </c>
       <c r="B26">
-        <v>202</v>
+        <v>230</v>
       </c>
       <c r="C26">
         <v>5</v>
@@ -2317,7 +2318,7 @@
         <v>43862</v>
       </c>
       <c r="B27">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C27">
         <v>4</v>
@@ -2328,7 +2329,7 @@
         <v>43891</v>
       </c>
       <c r="B28">
-        <v>260</v>
+        <v>157</v>
       </c>
       <c r="C28">
         <v>4</v>
@@ -2339,7 +2340,7 @@
         <v>43922</v>
       </c>
       <c r="B29">
-        <v>39</v>
+        <v>72</v>
       </c>
       <c r="C29">
         <v>1</v>
@@ -2350,7 +2351,7 @@
         <v>43952</v>
       </c>
       <c r="B30">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C30">
         <v>4</v>
@@ -2361,7 +2362,7 @@
         <v>43983</v>
       </c>
       <c r="B31">
-        <v>88</v>
+        <v>43</v>
       </c>
       <c r="C31">
         <v>6</v>
@@ -2372,7 +2373,7 @@
         <v>44013</v>
       </c>
       <c r="B32">
-        <v>236</v>
+        <v>108</v>
       </c>
       <c r="C32">
         <v>4</v>
@@ -2383,7 +2384,7 @@
         <v>44044</v>
       </c>
       <c r="B33">
-        <v>145</v>
+        <v>230</v>
       </c>
       <c r="C33">
         <v>6</v>
@@ -2394,7 +2395,7 @@
         <v>44075</v>
       </c>
       <c r="B34">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="C34">
         <v>6</v>
@@ -2405,10 +2406,10 @@
         <v>44105</v>
       </c>
       <c r="B35">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="C35">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
@@ -2416,7 +2417,7 @@
         <v>44136</v>
       </c>
       <c r="B36">
-        <v>194</v>
+        <v>123</v>
       </c>
       <c r="C36">
         <v>4</v>
@@ -2430,7 +2431,7 @@
         <v>126</v>
       </c>
       <c r="C37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
@@ -2438,7 +2439,7 @@
         <v>44197</v>
       </c>
       <c r="B38">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="C38">
         <v>2</v>
@@ -2449,7 +2450,7 @@
         <v>44228</v>
       </c>
       <c r="B39">
-        <v>121</v>
+        <v>127</v>
       </c>
       <c r="C39">
         <v>6</v>
@@ -2460,7 +2461,7 @@
         <v>44256</v>
       </c>
       <c r="B40">
-        <v>129</v>
+        <v>150</v>
       </c>
       <c r="C40">
         <v>5</v>
@@ -2482,7 +2483,7 @@
         <v>44317</v>
       </c>
       <c r="B42">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="C42">
         <v>5</v>
@@ -2493,7 +2494,7 @@
         <v>44348</v>
       </c>
       <c r="B43">
-        <v>339</v>
+        <v>207</v>
       </c>
       <c r="C43">
         <v>8</v>
@@ -2504,7 +2505,7 @@
         <v>44378</v>
       </c>
       <c r="B44">
-        <v>315</v>
+        <v>236</v>
       </c>
       <c r="C44">
         <v>7</v>
@@ -2515,10 +2516,10 @@
         <v>44409</v>
       </c>
       <c r="B45">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C45">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
@@ -2526,7 +2527,7 @@
         <v>44440</v>
       </c>
       <c r="B46">
-        <v>225</v>
+        <v>205</v>
       </c>
       <c r="C46">
         <v>7</v>
@@ -2537,7 +2538,7 @@
         <v>44470</v>
       </c>
       <c r="B47">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="C47">
         <v>4</v>
@@ -2548,7 +2549,7 @@
         <v>44501</v>
       </c>
       <c r="B48">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -2559,7 +2560,7 @@
         <v>44531</v>
       </c>
       <c r="B49">
-        <v>123</v>
+        <v>204</v>
       </c>
       <c r="C49">
         <v>4</v>
@@ -2570,10 +2571,10 @@
         <v>44562</v>
       </c>
       <c r="B50">
-        <v>98</v>
+        <v>141</v>
       </c>
       <c r="C50">
-        <v>27</v>
+        <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -2581,7 +2582,7 @@
         <v>44593</v>
       </c>
       <c r="B51">
-        <v>209</v>
+        <v>180</v>
       </c>
       <c r="C51">
         <v>10</v>

</xml_diff>